<commit_message>
13.07.2020 Mugdho Corporation Sales Details
</commit_message>
<xml_diff>
--- a/2020/Requisition/13.01.2020 Requisition of Mughdo Corporation.xlsx
+++ b/2020/Requisition/13.01.2020 Requisition of Mughdo Corporation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\Requisition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F263325F-809D-42D7-9CD6-99C478B4D308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90C932E-38A6-46AD-AE87-1ECE3F31F89E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="1080" windowWidth="11265" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Requisition" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="129">
   <si>
     <t>Model Name</t>
   </si>
@@ -421,6 +421,15 @@
   </si>
   <si>
     <t>13.01.2020</t>
+  </si>
+  <si>
+    <t>Only Black_Purple_Blue</t>
+  </si>
+  <si>
+    <t>Only Black_Crnberry_Blue</t>
+  </si>
+  <si>
+    <t>DrakBlue &amp; Gold</t>
   </si>
 </sst>
 </file>
@@ -506,7 +515,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -534,6 +543,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -612,7 +627,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -725,6 +740,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1075,7 +1093,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A99" sqref="A99"/>
+      <selection pane="bottomRight" activeCell="I105" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -2283,14 +2301,14 @@
         <v>4885.6000000000004</v>
       </c>
       <c r="C33" s="8">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D33" s="10">
         <f t="shared" si="0"/>
-        <v>48856</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>92</v>
+        <v>146568</v>
+      </c>
+      <c r="E33" s="48" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
@@ -2400,14 +2418,14 @@
         <v>5412.5</v>
       </c>
       <c r="C36" s="8">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="D36" s="10">
         <f>C36*B36</f>
-        <v>211087.5</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>92</v>
+        <v>378875</v>
+      </c>
+      <c r="E36" s="48" t="s">
+        <v>126</v>
       </c>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>
@@ -2940,14 +2958,14 @@
         <v>4174.41</v>
       </c>
       <c r="C67" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D67" s="10">
         <f t="shared" si="1"/>
-        <v>20872.05</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>92</v>
+        <v>16697.64</v>
+      </c>
+      <c r="E67" s="48" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
@@ -3501,19 +3519,17 @@
       <c r="BB86" s="32"/>
       <c r="BC86" s="32"/>
     </row>
-    <row r="87" spans="1:74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:74" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>116</v>
       </c>
       <c r="B87" s="9">
         <v>3520.36</v>
       </c>
-      <c r="C87" s="8">
-        <v>10</v>
-      </c>
+      <c r="C87" s="8"/>
       <c r="D87" s="10">
         <f t="shared" si="2"/>
-        <v>35203.599999999999</v>
+        <v>0</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>92</v>
@@ -3886,11 +3902,11 @@
       <c r="B95" s="44"/>
       <c r="C95" s="16">
         <f>SUBTOTAL(9,C7:C94)</f>
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="D95" s="17">
         <f>SUBTOTAL(9,D7:D94)</f>
-        <v>316019.14999999997</v>
+        <v>542140.64</v>
       </c>
       <c r="E95" s="31"/>
       <c r="F95" s="33"/>
@@ -4047,7 +4063,7 @@
         <v>22</v>
       </c>
       <c r="C100" s="21">
-        <v>300000</v>
+        <v>340000</v>
       </c>
       <c r="D100" s="8"/>
       <c r="G100" s="39"/>
@@ -4100,7 +4116,7 @@
       </c>
       <c r="C104" s="22">
         <f>SUBTOTAL(9,C99:C103)</f>
-        <v>300000</v>
+        <v>340000</v>
       </c>
       <c r="D104" s="15"/>
       <c r="E104" s="23"/>

</xml_diff>